<commit_message>
aact-902:  Add proj-tag-moc (Main publication that uses Mental, Oncology & Cardiology terms)
</commit_message>
<xml_diff>
--- a/public/incoming/originals/AACTProjects_20190307.xlsx
+++ b/public/incoming/originals/AACTProjects_20190307.xlsx
@@ -28,64 +28,17 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="111">
   <si>
+    <t xml:space="preserve">Our analysis was restricted to interventional studies registered with ClinicalTrials.gov between October 2007 and September 2010. To identify interventional studies, we used studies.study_type which provides the following choices: interventional, observational, expanded access, and not available (NA). Interventional studies were regrouped within the downloaded, derivative database according to the 3 clinical specialties—cardiovascular, oncology, and mental health. For this regrouping, we used submitted disease condition terms and Medical Subject Heading (MeSH) terms generated by a National Library of Medicine (NLM) algorithm to develop a methodology to annotate, validate, adjudicate, and implement disease condition terms (MeSH and non-MeSH) to create specialty data sets.
+A subset of the 2010 MeSH thesaurus from the NLM21 and a list of non-MeSH disease condition terms provided by data submitters that appeared in 5 or more interventional studies in the analysis data set were reviewed and annotated by clinical specialists at Duke University Medical Center. Terms were annotated according to their relevance to a given specialty (Y = relevant, N = not relevant). Specialty data sets were created and the results of algorithmic classifications were validated by comparison with classifications based on manual review. Clinical trials were classed according to date registered and by interventional status. 
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1001/jama.2012.3424</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>analyzed study counts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Because we could not precisely identify which applicable clinical trials are subject to FDAAA provisions using publicly available data, we used an algorithm that is based on input from the National Library of Medicine (Zarin D: personal communication) to identify 32,656 highly likely applicable clinical trials (HLACTs) from among all registered trials (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="62"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Table S1 in the Supplementary Appendix</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, available with the full text of this article at NEJM.org). We further restricted our study to HLACTs with a recruitment status of “completed” or “terminated” before August 31, 2012, to allow at least 1 year of reporting for trials with a primary completion date of September 2012. We excluded 1131 trials for which dates of trial completion could not be determined and for which the date of the last data verification was either before 2008 (1078 trials) or after September 2012 (53 trials). Our final study population included 13,327 HLACTs that had been either completed or terminated between January 1, 2008, and August 31, 2012 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="62"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Fig. 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>). To estimate rates of false positive and false negative findings, we also conducted a manual review of random samples of HLACTs and non-HLACTs (see </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="62"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Tables S15A and S15B in the Supplementary Appendix</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t> for details). To determine whether a product or indication was approved by the FDA (and if approved, the approval date), we searched Drugs@FDA, the National Drug Code Directory (for generics and supplements), the 510(k) Premarket Notification database (for devices), the Premarket Approval database (for devices), and Biologic Approvals by Year database and also conducted Web searches when necessary. Two of the authors manually reviewed uncertain cases to provide high and low estimates for false positives and false negatives.</t>
-    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -550,9 +503,6 @@
     <t>10.1542/peds.2011-3565</t>
   </si>
   <si>
-    <t>10.1001/jama.2012.3424</t>
-  </si>
-  <si>
     <t>PMC3882749</t>
   </si>
   <si>
@@ -639,7 +589,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,11 +681,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="62"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -894,7 +839,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1037,14 +982,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1330,10 +1278,10 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="L15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1354,17 +1302,17 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="28">
       <c r="A2" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>102</v>
@@ -1372,7 +1320,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4">
         <v>43479</v>
@@ -1384,31 +1332,31 @@
     </row>
     <row r="6" spans="1:13" ht="28">
       <c r="A6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>92</v>
@@ -1417,21 +1365,21 @@
         <v>93</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="34" customFormat="1" ht="224">
       <c r="A7" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" s="32">
         <v>26360527</v>
@@ -1449,30 +1397,30 @@
       <c r="K7" s="32"/>
       <c r="L7" s="32"/>
       <c r="M7" s="32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="37" customFormat="1" ht="210">
       <c r="A8" s="35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="35">
         <v>25239436</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
@@ -1480,18 +1428,18 @@
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
       <c r="M8" s="46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="37" customFormat="1" ht="70">
       <c r="A9" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="35">
         <v>23987571</v>
@@ -1512,20 +1460,20 @@
     </row>
     <row r="10" spans="1:13" s="40" customFormat="1" ht="56">
       <c r="A10" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="38">
         <v>24146958</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
@@ -1537,13 +1485,13 @@
     </row>
     <row r="11" spans="1:13" s="37" customFormat="1" ht="70">
       <c r="A11" s="35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="35">
         <v>24107478</v>
@@ -1567,19 +1515,19 @@
         <v>110</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="35">
         <v>24072529</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G12" s="35"/>
       <c r="H12" s="35"/>
@@ -1591,10 +1539,10 @@
     </row>
     <row r="13" spans="1:13" s="37" customFormat="1" ht="70">
       <c r="A13" s="35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="35">
@@ -1602,7 +1550,7 @@
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G13" s="35"/>
       <c r="H13" s="35"/>
@@ -1614,10 +1562,10 @@
     </row>
     <row r="14" spans="1:13" s="37" customFormat="1" ht="42">
       <c r="A14" s="35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="35"/>
       <c r="D14" s="35"/>
@@ -1633,10 +1581,10 @@
     </row>
     <row r="15" spans="1:13" s="37" customFormat="1" ht="42">
       <c r="A15" s="35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="35"/>
@@ -1652,22 +1600,22 @@
     </row>
     <row r="16" spans="1:13" s="37" customFormat="1" ht="56">
       <c r="A16" s="35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D16" s="35">
         <v>23027172</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
@@ -1677,31 +1625,33 @@
       <c r="L16" s="35"/>
       <c r="M16" s="35"/>
     </row>
-    <row r="17" spans="1:13" s="49" customFormat="1" ht="168">
+    <row r="17" spans="1:13" s="48" customFormat="1" ht="196">
       <c r="A17" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="47" t="s">
         <v>3</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>2</v>
       </c>
       <c r="D17" s="47">
         <v>22550198</v>
       </c>
       <c r="E17" s="47"/>
-      <c r="F17" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="47"/>
+      <c r="F17" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="50">
+        <v>40448</v>
+      </c>
       <c r="H17" s="47"/>
       <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="47"/>
       <c r="L17" s="47"/>
-      <c r="M17" s="50" t="s">
-        <v>1</v>
+      <c r="M17" s="49" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="37" customFormat="1" ht="140">
@@ -1709,10 +1659,10 @@
         <v>97</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D18" s="35">
         <v>24890544</v>
@@ -1736,10 +1686,10 @@
         <v>101</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="2">
         <v>30158197</v>
@@ -1750,48 +1700,49 @@
     </row>
     <row r="20" spans="1:13" ht="364">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" s="2">
         <v>27191848</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G20" s="44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M20" s="43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="126">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" s="2">
         <v>23564296</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <autoFilter ref="A6:L6"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
@@ -1840,19 +1791,19 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="281" thickBot="1">
       <c r="A1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="C1" s="9">
         <v>25760355</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" s="11">
         <v>41544</v>
@@ -1875,10 +1826,10 @@
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="336">
       <c r="A2" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="16">
         <v>24315119</v>
@@ -1899,10 +1850,10 @@
         <v>96</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>95</v>
@@ -1910,7 +1861,7 @@
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="210">
       <c r="A3" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1921,13 +1872,13 @@
         <v>91</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K3" s="24" t="s">
         <v>95</v>
@@ -1935,7 +1886,7 @@
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="351" thickBot="1">
       <c r="A4" s="25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -1946,16 +1897,16 @@
         <v>94</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J4" s="30" t="s">
         <v>106</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>